<commit_message>
Cau 03 Va Cau 04 v2
</commit_message>
<xml_diff>
--- a/wwwroot/data/DanhSach.xlsx
+++ b/wwwroot/data/DanhSach.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChuyenNganh2025\HocKy5\ASP_Core\23WebC_Nhom10\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EACB187-B216-4AAD-A12C-59F9C650B9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E39D800-D658-4763-89BB-B07A30377992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F96C799F-20F9-47F1-869E-54A6B6C363BA}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{F96C799F-20F9-47F1-869E-54A6B6C363BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,72 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>12321ádfasfdfsf</t>
+  </si>
+  <si>
+    <t>adsfdsfsda</t>
+  </si>
+  <si>
+    <t>ấdfsavdfv</t>
+  </si>
+  <si>
+    <t>vxzvczx</t>
+  </si>
+  <si>
+    <t>zcxvxczv</t>
+  </si>
+  <si>
+    <t>agfdgfadg</t>
+  </si>
+  <si>
+    <t>gadgfag</t>
+  </si>
+  <si>
+    <t>fdgagfd</t>
+  </si>
+  <si>
+    <t>àdgfda</t>
+  </si>
+  <si>
+    <t>fadg</t>
+  </si>
+  <si>
+    <t>sdfgdfs</t>
   </si>
 </sst>
 </file>
@@ -108,9 +174,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -426,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC953504-DCC8-49F2-8FE0-05704FA800C4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +574,127 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4D20B77E-A399-424C-9932-126CF2B97950}"/>

</xml_diff>